<commit_message>
Tweak naming of timeline
</commit_message>
<xml_diff>
--- a/test_data/CDISC_Pilot_Study_VS_Timeline.xlsx
+++ b/test_data/CDISC_Pilot_Study_VS_Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBF238E-A1B5-CC46-91A6-B79F4231B738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA4FC8F-4F7B-754D-9824-C5E91AB6960D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26820" yWindow="500" windowWidth="61200" windowHeight="27240" activeTab="7" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="26820" yWindow="500" windowWidth="61200" windowHeight="27240" activeTab="10" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="775">
   <si>
     <t>Screening</t>
   </si>
@@ -2397,6 +2397,15 @@
   </si>
   <si>
     <t>BC:Body temperature, BC:Body Weight, BC:Body Height, TL: vsBloodPressure</t>
+  </si>
+  <si>
+    <t>Vital Sign Blood Pressure Timeline</t>
+  </si>
+  <si>
+    <t>BP Profile</t>
+  </si>
+  <si>
+    <t>Automatic execution</t>
   </si>
 </sst>
 </file>
@@ -2630,13 +2639,13 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3618,8 +3627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A98DD9-8159-D74D-B42C-CCC2F4D10811}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3635,7 +3644,7 @@
         <v>85</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>699</v>
+        <v>772</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>233</v>
@@ -3658,7 +3667,7 @@
         <v>87</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>694</v>
+        <v>773</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>37</v>
@@ -3670,7 +3679,7 @@
         <v>89</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>695</v>
+        <v>774</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>508</v>
@@ -7571,120 +7580,120 @@
       <c r="A1" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="51" t="s">
         <v>696</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="51" t="s">
         <v>731</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -7776,16 +7785,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8128,7 +8137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:V68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C24" sqref="C24:C25"/>
     </sheetView>
   </sheetViews>
@@ -11408,6 +11417,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -11608,27 +11637,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11645,29 +11679,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Tweak to test file and code
</commit_message>
<xml_diff>
--- a/test_data/CDISC_Pilot_Study_VS_Timeline.xlsx
+++ b/test_data/CDISC_Pilot_Study_VS_Timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA4FC8F-4F7B-754D-9824-C5E91AB6960D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F06042-6567-A84B-8A1B-EE2C52000F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26820" yWindow="500" windowWidth="61200" windowHeight="27240" activeTab="10" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="26920" yWindow="500" windowWidth="47700" windowHeight="27240" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="777">
   <si>
     <t>Screening</t>
   </si>
@@ -1598,9 +1598,6 @@
     <t>study_version</t>
   </si>
   <si>
-    <t>Approval</t>
-  </si>
-  <si>
     <t>Design approval date</t>
   </si>
   <si>
@@ -1656,9 +1653,6 @@
   </si>
   <si>
     <t>IRB/IEC Feedback</t>
-  </si>
-  <si>
-    <t>Region: Europe=15, Country: USA=20%</t>
   </si>
   <si>
     <t>Other=Fix typographical errors</t>
@@ -2406,6 +2400,18 @@
   </si>
   <si>
     <t>Automatic execution</t>
+  </si>
+  <si>
+    <t>D_APPROVE</t>
+  </si>
+  <si>
+    <t>P_APPROVE</t>
+  </si>
+  <si>
+    <t>Region: Europe=15</t>
+  </si>
+  <si>
+    <t>LZZT</t>
   </si>
 </sst>
 </file>
@@ -2963,8 +2969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E79CD3-D94C-A14B-9EDC-9C26AFA63552}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2983,7 +2989,7 @@
         <v>233</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E1" s="41"/>
       <c r="F1" s="41"/>
@@ -3033,7 +3039,7 @@
         <v>68</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>207</v>
+        <v>776</v>
       </c>
       <c r="E6" s="41"/>
       <c r="F6" s="41"/>
@@ -3147,46 +3153,46 @@
       <c r="A17" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" t="s">
+        <v>773</v>
+      </c>
+      <c r="C17" t="s">
         <v>512</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>513</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>514</v>
       </c>
-      <c r="E17" t="s">
-        <v>515</v>
-      </c>
       <c r="F17" s="43">
-        <v>38899</v>
+        <v>38869</v>
       </c>
       <c r="G17" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
+        <v>515</v>
+      </c>
+      <c r="B18" t="s">
+        <v>774</v>
+      </c>
+      <c r="C18" t="s">
         <v>516</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>512</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>517</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>518</v>
-      </c>
-      <c r="E18" t="s">
-        <v>519</v>
       </c>
       <c r="F18" s="43">
         <v>38899</v>
       </c>
       <c r="G18" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
   </sheetData>
@@ -3217,13 +3223,13 @@
         <v>85</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>233</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3231,7 +3237,7 @@
         <v>87</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>37</v>
@@ -3245,13 +3251,13 @@
         <v>89</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>508</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3261,38 +3267,38 @@
         <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="17" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="17" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="17" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="17" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3319,7 +3325,7 @@
     <row r="11" spans="1:4" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="3" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>209</v>
@@ -3364,7 +3370,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>1</v>
@@ -3383,7 +3389,7 @@
     <row r="17" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="6" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="1" t="s">
@@ -3393,7 +3399,7 @@
     <row r="18" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="1" t="s">
@@ -3455,10 +3461,10 @@
     <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
       <c r="B24" s="3" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>1</v>
@@ -3627,7 +3633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A98DD9-8159-D74D-B42C-CCC2F4D10811}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -3644,22 +3650,22 @@
         <v>85</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>233</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3667,7 +3673,7 @@
         <v>87</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>37</v>
@@ -3679,22 +3685,22 @@
         <v>89</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>508</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>738</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -3704,56 +3710,56 @@
         <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="17" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="17" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="17" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="17" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -3770,10 +3776,10 @@
     <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="3" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>1</v>
@@ -3782,10 +3788,10 @@
     <row r="11" spans="1:7" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="3" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>1</v>
@@ -3794,10 +3800,10 @@
     <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="3" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>1</v>
@@ -3806,10 +3812,10 @@
     <row r="13" spans="1:7" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>1</v>
@@ -3975,620 +3981,620 @@
         <v>36</v>
       </c>
       <c r="E1" s="44" t="s">
+        <v>537</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>538</v>
+      </c>
+      <c r="G1" s="44" t="s">
         <v>539</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="H1" s="44" t="s">
         <v>540</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="I1" s="44" t="s">
         <v>541</v>
-      </c>
-      <c r="H1" s="44" t="s">
-        <v>542</v>
-      </c>
-      <c r="I1" s="44" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>546</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>548</v>
       </c>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>551</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>569</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>556</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>557</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>558</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>144</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>145</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>213</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>154</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>155</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>156</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>157</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>158</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="41" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="41" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>733</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>735</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I23" s="1"/>
     </row>
@@ -4626,10 +4632,10 @@
         <v>508</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -4657,18 +4663,18 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="C7" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -4703,10 +4709,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C14" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -4756,7 +4762,7 @@
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -4766,10 +4772,10 @@
     </row>
     <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -4804,39 +4810,39 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
+        <v>753</v>
+      </c>
+      <c r="C34" t="s">
         <v>755</v>
-      </c>
-      <c r="C34" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C35" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="C36" t="s">
         <v>756</v>
-      </c>
-      <c r="C36" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C37" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
   </sheetData>
@@ -4879,7 +4885,7 @@
         <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C2" t="s">
         <v>226</v>
@@ -4893,7 +4899,7 @@
         <v>227</v>
       </c>
       <c r="B3" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C3" t="s">
         <v>226</v>
@@ -4947,7 +4953,7 @@
     </row>
     <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>206</v>
@@ -4996,34 +5002,34 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>45</v>
       </c>
       <c r="C1" s="21" t="s">
+        <v>611</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>613</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>615</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>46</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>47</v>
       </c>
       <c r="H1" s="21" t="s">
+        <v>612</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>680</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>614</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>682</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>616</v>
       </c>
       <c r="K1" s="21" t="s">
         <v>48</v>
@@ -5036,11 +5042,11 @@
         <v>62</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>50</v>
@@ -5082,10 +5088,10 @@
         <v>63</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>50</v>
@@ -5144,11 +5150,11 @@
         <v>179</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="16" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>51</v>
@@ -5497,25 +5503,25 @@
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="31" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
   </sheetData>
@@ -5558,10 +5564,10 @@
         <v>36</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>98</v>
@@ -5593,7 +5599,7 @@
         <v>104</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5722,7 +5728,7 @@
         <v>141</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -5742,7 +5748,7 @@
         <v>141</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -5762,7 +5768,7 @@
         <v>141</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -5782,7 +5788,7 @@
         <v>141</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -5839,7 +5845,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A36B6E2-81ED-B543-A330-D9502D2DF96E}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5853,22 +5861,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
+        <v>522</v>
+      </c>
+      <c r="B1" s="42" t="s">
         <v>523</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="C1" s="42" t="s">
         <v>524</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="D1" s="42" t="s">
         <v>525</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="E1" s="42" t="s">
         <v>526</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="F1" s="45" t="s">
         <v>527</v>
-      </c>
-      <c r="F1" s="45" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -5876,19 +5884,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>528</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>529</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="14" t="s">
         <v>530</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="14" t="s">
         <v>531</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>533</v>
-      </c>
       <c r="F2" s="14" t="s">
-        <v>532</v>
+        <v>775</v>
       </c>
     </row>
   </sheetData>
@@ -5983,7 +5991,7 @@
         <v>187</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>183</v>
@@ -5997,7 +6005,7 @@
         <v>190</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D6" s="46" t="s">
         <v>189</v>
@@ -6011,7 +6019,7 @@
         <v>187</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D7" s="46" t="s">
         <v>191</v>
@@ -6025,7 +6033,7 @@
         <v>123</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D8" s="47" t="s">
         <v>193</v>
@@ -6069,36 +6077,36 @@
         <v>508</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>60</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B2" t="s">
+        <v>603</v>
+      </c>
+      <c r="C2" t="s">
+        <v>604</v>
+      </c>
+      <c r="D2" t="s">
         <v>605</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>606</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>607</v>
-      </c>
-      <c r="E2" t="s">
-        <v>608</v>
-      </c>
-      <c r="F2" t="s">
-        <v>609</v>
       </c>
       <c r="G2" t="s">
         <v>41</v>
@@ -6106,13 +6114,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="E3" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="F3" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="G3" t="s">
         <v>42</v>
@@ -6120,13 +6128,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="E4" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="F4" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="G4" t="s">
         <v>39</v>
@@ -6134,22 +6142,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>706</v>
+      </c>
+      <c r="B5" t="s">
+        <v>707</v>
+      </c>
+      <c r="C5" t="s">
         <v>708</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>709</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
+        <v>577</v>
+      </c>
+      <c r="F5" t="s">
         <v>710</v>
-      </c>
-      <c r="D5" t="s">
-        <v>711</v>
-      </c>
-      <c r="E5" t="s">
-        <v>579</v>
-      </c>
-      <c r="F5" t="s">
-        <v>712</v>
       </c>
       <c r="G5" t="s">
         <v>508</v>
@@ -6199,7 +6207,7 @@
         <v>506</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6275,7 +6283,7 @@
         <v>503</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6312,7 +6320,7 @@
         <v>259</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="68" customHeight="1" x14ac:dyDescent="0.2">
@@ -6324,7 +6332,7 @@
         <v>261</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -6381,7 +6389,7 @@
         <v>273</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -6402,7 +6410,7 @@
         <v>277</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6414,7 +6422,7 @@
         <v>279</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6444,7 +6452,7 @@
         <v>285</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -7531,24 +7539,24 @@
         <v>207</v>
       </c>
       <c r="F2" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>532</v>
+      </c>
+      <c r="B3" t="s">
+        <v>533</v>
+      </c>
+      <c r="C3" t="s">
         <v>534</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>535</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>536</v>
-      </c>
-      <c r="D3" t="s">
-        <v>537</v>
-      </c>
-      <c r="E3" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -7653,7 +7661,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C7" s="49"/>
       <c r="D7" s="49"/>
@@ -7689,7 +7697,7 @@
         <v>84</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C10" s="51"/>
       <c r="D10" s="51"/>
@@ -7725,7 +7733,7 @@
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>118</v>
@@ -7826,7 +7834,7 @@
         <v>507</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C1" s="21" t="s">
         <v>233</v>
@@ -7841,84 +7849,84 @@
         <v>235</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
+        <v>594</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>595</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>596</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="D2" s="14" t="s">
         <v>597</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="F2" s="16" t="s">
         <v>598</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>599</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>600</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B3" s="40" t="s">
+        <v>712</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>713</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>714</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="F3" s="16" t="s">
         <v>715</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>716</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>717</v>
-      </c>
       <c r="G3" s="14" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B4" s="40" t="s">
+        <v>716</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>717</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>718</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="F4" s="16" t="s">
         <v>719</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>720</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>721</v>
-      </c>
       <c r="G4" s="14" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
+        <v>724</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>725</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>727</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>728</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>726</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>727</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>729</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>730</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>728</v>
       </c>
     </row>
   </sheetData>
@@ -7957,10 +7965,10 @@
         <v>36</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8080,7 +8088,7 @@
         <v>222</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>136</v>
@@ -8094,7 +8102,7 @@
         <v>222</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>136</v>
@@ -8108,7 +8116,7 @@
         <v>222</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>136</v>
@@ -8122,7 +8130,7 @@
         <v>224</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>225</v>
@@ -8172,52 +8180,52 @@
         <v>233</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>634</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>635</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>576</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="10" t="s">
         <v>639</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -8290,13 +8298,13 @@
         <v>508</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>144</v>
@@ -8311,25 +8319,25 @@
         <v>213</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>154</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>155</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>156</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>157</v>
@@ -8345,121 +8353,121 @@
         <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="17" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="L5" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>634</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="P5" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>635</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>576</v>
-      </c>
-      <c r="P5" s="1" t="s">
+      <c r="R5" s="10" t="s">
         <v>639</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>641</v>
-      </c>
       <c r="S5" s="2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="17" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="17" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>0</v>
@@ -8514,7 +8522,7 @@
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="17" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>100</v>
@@ -8799,7 +8807,7 @@
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="3" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="1" t="s">
@@ -8854,7 +8862,7 @@
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="3" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="1" t="s">
@@ -9239,10 +9247,10 @@
     <row r="22" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="3" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>1</v>
@@ -9519,7 +9527,7 @@
         <v>169</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>1</v>
@@ -9686,7 +9694,7 @@
         <v>13</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>1</v>
@@ -9795,7 +9803,7 @@
     <row r="32" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
       <c r="B32" s="6" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="30" t="s">
@@ -9907,7 +9915,7 @@
     <row r="34" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
       <c r="B34" s="6" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="1" t="s">
@@ -10701,13 +10709,13 @@
         <v>85</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>233</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="17" x14ac:dyDescent="0.2">
@@ -10715,7 +10723,7 @@
         <v>87</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>37</v>
@@ -10729,13 +10737,13 @@
         <v>89</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>508</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
@@ -10745,38 +10753,38 @@
         <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="17" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="17" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="17" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="17" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update Pilot test file
</commit_message>
<xml_diff>
--- a/test_data/CDISC_Pilot_Study_VS_Timeline.xlsx
+++ b/test_data/CDISC_Pilot_Study_VS_Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEBB730-A752-FC44-924A-AB88E7F71CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF06886-2ECE-BE47-88B5-460711CAFC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26920" yWindow="500" windowWidth="47700" windowHeight="27240" firstSheet="10" activeTab="21" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="26920" yWindow="500" windowWidth="47700" windowHeight="27240" firstSheet="10" activeTab="19" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="793">
   <si>
     <t>Screening</t>
   </si>
@@ -2694,13 +2694,13 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4003,7 +4003,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5755,10 +5755,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB4E9D5-B601-284A-9651-0AA604C2B9D1}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5773,7 +5773,7 @@
     <col min="8" max="8" width="61.6640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>230</v>
       </c>
@@ -5798,8 +5798,11 @@
       <c r="H1" s="21" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I1" s="21" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>97</v>
       </c>
@@ -5825,7 +5828,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>102</v>
       </c>
@@ -5847,8 +5850,11 @@
       <c r="H3" s="6" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I3" s="3" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>103</v>
       </c>
@@ -5874,7 +5880,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>105</v>
       </c>
@@ -5893,8 +5899,11 @@
       <c r="F5" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="3" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>106</v>
       </c>
@@ -5913,8 +5922,11 @@
       <c r="F6" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="3" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>107</v>
       </c>
@@ -5933,8 +5945,11 @@
       <c r="F7" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="3" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>108</v>
       </c>
@@ -5953,8 +5968,11 @@
       <c r="F8" s="3" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="3" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>109</v>
       </c>
@@ -5973,8 +5991,11 @@
       <c r="F9" s="3" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="3" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>110</v>
       </c>
@@ -5993,8 +6014,11 @@
       <c r="F10" s="3" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="3" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>112</v>
       </c>
@@ -6013,8 +6037,11 @@
       <c r="F11" s="3" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="3" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>113</v>
       </c>
@@ -6033,8 +6060,11 @@
       <c r="F12" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I12" s="3" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>114</v>
       </c>
@@ -6055,6 +6085,9 @@
       </c>
       <c r="H13" s="6" t="s">
         <v>111</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>586</v>
       </c>
     </row>
   </sheetData>
@@ -6212,7 +6245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989384DC-1C54-514A-8A1E-ADD84D891BA4}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -7748,120 +7781,120 @@
       <c r="A1" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="51" t="s">
         <v>202</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="49" t="s">
         <v>690</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="49" t="s">
         <v>725</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -7953,16 +7986,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11585,6 +11618,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
@@ -11593,15 +11635,6 @@
     <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11806,6 +11839,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11818,14 +11859,6 @@
     <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>